<commit_message>
trying to fix commit issue on new wfps regridding
</commit_message>
<xml_diff>
--- a/figs/202410_FirstRuns/res.xlsx
+++ b/figs/202410_FirstRuns/res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harris/Dropbox/UniBern_work/Applications_Proposals_Collabs/2024_ArcticIsoTONE/isotone_arcticBranch/figs/202410_FirstRuns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B23C31C-8060-BB48-B558-3172C104369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A5949-9E79-2647-A37C-52BAF4516684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4660" windowWidth="21520" windowHeight="13700" xr2:uid="{7E83D969-1CBA-C344-9BED-F32A59FFE65D}"/>
+    <workbookView xWindow="5440" yWindow="3700" windowWidth="21520" windowHeight="13700" xr2:uid="{7E83D969-1CBA-C344-9BED-F32A59FFE65D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Global run, Arctic mask</t>
   </si>
   <si>
-    <t>Flux, 1850</t>
-  </si>
-  <si>
     <t>Flux, 2020</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>TgN y-1</t>
+  </si>
+  <si>
+    <t>Flux, 1860</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,26 +503,26 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -533,10 +533,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.38</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D7">
-        <v>0.76</v>
+        <v>1.9</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -547,10 +547,10 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>2.9</v>
+        <v>4.3</v>
       </c>
       <c r="D8">
-        <v>5.4</v>
+        <v>7.2</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -558,26 +558,35 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>5.3</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>14.1</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>14.2</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -587,6 +596,12 @@
       <c r="B12" t="s">
         <v>0</v>
       </c>
+      <c r="C12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
@@ -601,26 +616,26 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>